<commit_message>
update data incl AAQ sites
</commit_message>
<xml_diff>
--- a/Data/data-lake/MWH/MWH_DigitisedData.xlsx
+++ b/Data/data-lake/MWH/MWH_DigitisedData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthipsey/Local/lake-richmond/Data/data-lake/MWH/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA74F5B-742A-F841-914A-861B99578A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25BF506-94B9-5C46-BB92-B4F5ABE97A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="700" windowWidth="33580" windowHeight="21140" xr2:uid="{94915F9F-3861-584A-B232-7A32DC8FEA4C}"/>
+    <workbookView xWindow="-41780" yWindow="3040" windowWidth="33580" windowHeight="21140" activeTab="1" xr2:uid="{94915F9F-3861-584A-B232-7A32DC8FEA4C}"/>
   </bookViews>
   <sheets>
     <sheet name="MWH lake RuchmondStadia" sheetId="8" r:id="rId1"/>
@@ -464,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB41793-2F04-0345-8136-52E318768742}">
   <dimension ref="A1:G260"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="G250" sqref="G250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3729,10 +3729,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{434DAC10-D998-7543-BBFE-D426EA13D353}">
-  <dimension ref="A1:Q53"/>
+  <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G39" sqref="G39:H54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3757,1376 +3757,1376 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>25.078538999999999</v>
-      </c>
-      <c r="B2">
-        <v>-0.18805053999999999</v>
-      </c>
-      <c r="D2">
-        <v>24.264278000000001</v>
-      </c>
-      <c r="E2">
-        <v>-0.13318029000000001</v>
-      </c>
-      <c r="G2">
-        <v>24.589797999999998</v>
-      </c>
-      <c r="H2">
-        <v>-0.29588072999999998</v>
-      </c>
-      <c r="J2">
-        <v>20.778587000000002</v>
-      </c>
-      <c r="K2">
-        <v>-0.40071318</v>
-      </c>
-      <c r="M2">
-        <v>17.651589999999999</v>
-      </c>
-      <c r="N2">
-        <v>-0.37082404000000002</v>
-      </c>
-      <c r="P2">
-        <v>15.567220000000001</v>
-      </c>
-      <c r="Q2">
-        <v>-0.12533327999999999</v>
-      </c>
-    </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>24.784424000000001</v>
+        <v>25.078538999999999</v>
       </c>
       <c r="B3">
-        <v>-0.91861550000000003</v>
+        <v>-0.18805053999999999</v>
       </c>
       <c r="D3">
-        <v>24.263359999999999</v>
+        <v>24.264278000000001</v>
       </c>
       <c r="E3">
-        <v>-0.83694195999999998</v>
+        <v>-0.13318029000000001</v>
       </c>
       <c r="G3">
-        <v>24.620992999999999</v>
+        <v>24.589797999999998</v>
       </c>
       <c r="H3">
-        <v>-1.3515526</v>
+        <v>-0.29588072999999998</v>
       </c>
       <c r="J3">
-        <v>20.777950000000001</v>
+        <v>20.778587000000002</v>
       </c>
       <c r="K3">
-        <v>-0.88793283999999995</v>
+        <v>-0.40071318</v>
       </c>
       <c r="M3">
-        <v>17.618416</v>
+        <v>17.651589999999999</v>
       </c>
       <c r="N3">
-        <v>-0.83094650000000003</v>
+        <v>-0.37082404000000002</v>
       </c>
       <c r="P3">
-        <v>15.729343</v>
+        <v>15.567220000000001</v>
       </c>
       <c r="Q3">
-        <v>-0.69390315000000002</v>
+        <v>-0.12533327999999999</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>24.392202000000001</v>
+        <v>24.784424000000001</v>
       </c>
       <c r="B4">
-        <v>-1.9468376999999999</v>
+        <v>-0.91861550000000003</v>
       </c>
       <c r="D4">
-        <v>24.229583999999999</v>
+        <v>24.263359999999999</v>
       </c>
       <c r="E4">
-        <v>-1.7572163000000001</v>
+        <v>-0.83694195999999998</v>
       </c>
       <c r="G4">
-        <v>24.522036</v>
+        <v>24.620992999999999</v>
       </c>
       <c r="H4">
-        <v>-2.2988360000000001</v>
+        <v>-1.3515526</v>
       </c>
       <c r="J4">
-        <v>20.809108999999999</v>
+        <v>20.777950000000001</v>
       </c>
       <c r="K4">
-        <v>-1.9706725</v>
+        <v>-0.88793283999999995</v>
       </c>
       <c r="M4">
-        <v>17.617107000000001</v>
+        <v>17.618416</v>
       </c>
       <c r="N4">
-        <v>-1.8324536</v>
+        <v>-0.83094650000000003</v>
       </c>
       <c r="P4">
-        <v>15.662924</v>
+        <v>15.729343</v>
       </c>
       <c r="Q4">
-        <v>-1.6682836000000001</v>
+        <v>-0.69390315000000002</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>23.706007</v>
+        <v>24.392202000000001</v>
       </c>
       <c r="B5">
-        <v>-3.5973537000000002</v>
+        <v>-1.9468376999999999</v>
       </c>
       <c r="D5">
-        <v>24.163128</v>
+        <v>24.229583999999999</v>
       </c>
       <c r="E5">
-        <v>-2.7586645999999999</v>
+        <v>-1.7572163000000001</v>
       </c>
       <c r="G5">
-        <v>24.325216000000001</v>
+        <v>24.522036</v>
       </c>
       <c r="H5">
-        <v>-3.3543021999999998</v>
+        <v>-2.2988360000000001</v>
       </c>
       <c r="J5">
-        <v>20.8078</v>
+        <v>20.809108999999999</v>
       </c>
       <c r="K5">
-        <v>-2.9721796999999999</v>
+        <v>-1.9706725</v>
       </c>
       <c r="M5">
-        <v>17.583224999999999</v>
+        <v>17.617107000000001</v>
       </c>
       <c r="N5">
-        <v>-2.8339311999999999</v>
+        <v>-1.8324536</v>
       </c>
       <c r="P5">
-        <v>15.661614999999999</v>
+        <v>15.662924</v>
       </c>
       <c r="Q5">
-        <v>-2.6697907000000001</v>
+        <v>-1.6682836000000001</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>22.237273999999999</v>
+        <v>23.706007</v>
       </c>
       <c r="B6">
-        <v>-5.8426549999999997</v>
+        <v>-3.5973537000000002</v>
       </c>
       <c r="D6">
-        <v>24.129352999999998</v>
+        <v>24.163128</v>
       </c>
       <c r="E6">
-        <v>-3.6789388999999999</v>
+        <v>-2.7586645999999999</v>
       </c>
       <c r="G6">
-        <v>23.704910000000002</v>
+        <v>24.325216000000001</v>
       </c>
       <c r="H6">
-        <v>-4.4364543000000003</v>
+        <v>-3.3543021999999998</v>
       </c>
       <c r="J6">
-        <v>20.383074000000001</v>
+        <v>20.8078</v>
       </c>
       <c r="K6">
-        <v>-3.9462367999999999</v>
+        <v>-2.9721796999999999</v>
       </c>
       <c r="M6">
-        <v>17.647027999999999</v>
+        <v>17.583224999999999</v>
       </c>
       <c r="N6">
-        <v>-3.8625647999999999</v>
+        <v>-2.8339311999999999</v>
       </c>
       <c r="P6">
-        <v>15.725453</v>
+        <v>15.661614999999999</v>
       </c>
       <c r="Q6">
-        <v>-3.6713564000000001</v>
+        <v>-2.6697907000000001</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>22.821435999999999</v>
+        <v>22.237273999999999</v>
       </c>
       <c r="B7">
-        <v>-7.4943169999999997</v>
+        <v>-5.8426549999999997</v>
       </c>
       <c r="D7">
-        <v>24.128008000000001</v>
+        <v>24.129352999999998</v>
       </c>
       <c r="E7">
-        <v>-4.7075139999999998</v>
+        <v>-3.6789388999999999</v>
       </c>
       <c r="G7">
-        <v>22.954487</v>
+        <v>23.704910000000002</v>
       </c>
       <c r="H7">
-        <v>-5.3831496000000003</v>
+        <v>-4.4364543000000003</v>
       </c>
       <c r="J7">
-        <v>20.251401999999999</v>
+        <v>20.383074000000001</v>
       </c>
       <c r="K7">
-        <v>-5.0017620000000003</v>
+        <v>-3.9462367999999999</v>
       </c>
       <c r="M7">
-        <v>17.613146</v>
+        <v>17.647027999999999</v>
       </c>
       <c r="N7">
-        <v>-4.8640423000000004</v>
+        <v>-3.8625647999999999</v>
       </c>
       <c r="P7">
-        <v>15.756682</v>
+        <v>15.725453</v>
       </c>
       <c r="Q7">
-        <v>-4.6999607000000001</v>
+        <v>-3.6713564000000001</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>22.396249999999998</v>
+        <v>22.821435999999999</v>
       </c>
       <c r="B8">
-        <v>-8.8202549999999995</v>
+        <v>-7.4943169999999997</v>
       </c>
       <c r="D8">
-        <v>24.061554000000001</v>
+        <v>24.128008000000001</v>
       </c>
       <c r="E8">
-        <v>-5.7089619999999996</v>
+        <v>-4.7075139999999998</v>
       </c>
       <c r="G8">
-        <v>22.823027</v>
+        <v>22.954487</v>
       </c>
       <c r="H8">
-        <v>-6.276268</v>
+        <v>-5.3831496000000003</v>
       </c>
       <c r="J8">
-        <v>20.282700999999999</v>
+        <v>20.251401999999999</v>
       </c>
       <c r="K8">
-        <v>-5.9762306000000001</v>
+        <v>-5.0017620000000003</v>
       </c>
       <c r="M8">
-        <v>17.611801</v>
+        <v>17.613146</v>
       </c>
       <c r="N8">
-        <v>-5.8926170000000004</v>
+        <v>-4.8640423000000004</v>
       </c>
       <c r="P8">
-        <v>15.722801</v>
+        <v>15.756682</v>
       </c>
       <c r="Q8">
-        <v>-5.7014383999999998</v>
+        <v>-4.6999607000000001</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>21.971665999999999</v>
+        <v>22.396249999999998</v>
       </c>
       <c r="B9">
-        <v>-9.6860420000000005</v>
+        <v>-8.8202549999999995</v>
       </c>
       <c r="D9">
-        <v>23.669401000000001</v>
+        <v>24.061554000000001</v>
       </c>
       <c r="E9">
-        <v>-6.6830486999999996</v>
+        <v>-5.7089619999999996</v>
       </c>
       <c r="G9">
-        <v>22.788969000000002</v>
+        <v>22.823027</v>
       </c>
       <c r="H9">
-        <v>-7.4130845000000001</v>
+        <v>-6.276268</v>
       </c>
       <c r="J9">
-        <v>20.34647</v>
+        <v>20.282700999999999</v>
       </c>
       <c r="K9">
-        <v>-7.0319320000000003</v>
+        <v>-5.9762306000000001</v>
       </c>
       <c r="M9">
-        <v>17.545347</v>
+        <v>17.611801</v>
       </c>
       <c r="N9">
-        <v>-6.8940653999999997</v>
+        <v>-5.8926170000000004</v>
       </c>
       <c r="P9">
-        <v>15.688884</v>
+        <v>15.722801</v>
       </c>
       <c r="Q9">
-        <v>-6.729984</v>
+        <v>-5.7014383999999998</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>21.644553999999999</v>
+        <v>21.971665999999999</v>
       </c>
       <c r="B10">
-        <v>-10.741390000000001</v>
+        <v>-9.6860420000000005</v>
       </c>
       <c r="D10">
-        <v>23.70063</v>
+        <v>23.669401000000001</v>
       </c>
       <c r="E10">
-        <v>-7.7116528000000004</v>
+        <v>-6.6830486999999996</v>
       </c>
       <c r="G10">
-        <v>22.559646999999998</v>
+        <v>22.788969000000002</v>
       </c>
       <c r="H10">
-        <v>-8.4143860000000004</v>
+        <v>-7.4130845000000001</v>
       </c>
       <c r="J10">
-        <v>20.084468999999999</v>
+        <v>20.34647</v>
       </c>
       <c r="K10">
-        <v>-8.1144069999999999</v>
+        <v>-7.0319320000000003</v>
       </c>
       <c r="M10">
-        <v>17.511465000000001</v>
+        <v>17.545347</v>
       </c>
       <c r="N10">
-        <v>-7.895543</v>
+        <v>-6.8940653999999997</v>
       </c>
       <c r="P10">
-        <v>15.785365000000001</v>
+        <v>15.688884</v>
       </c>
       <c r="Q10">
-        <v>-7.6774434999999999</v>
+        <v>-6.729984</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>21.513978999999999</v>
+        <v>21.644553999999999</v>
       </c>
       <c r="B11">
-        <v>-10.957814000000001</v>
+        <v>-10.741390000000001</v>
       </c>
       <c r="D11">
-        <v>23.048351</v>
+        <v>23.70063</v>
       </c>
       <c r="E11">
-        <v>-8.3336240000000004</v>
+        <v>-7.7116528000000004</v>
       </c>
       <c r="G11">
-        <v>22.265356000000001</v>
+        <v>22.559646999999998</v>
       </c>
       <c r="H11">
-        <v>-9.2802900000000008</v>
+        <v>-8.4143860000000004</v>
       </c>
       <c r="J11">
-        <v>20.180986000000001</v>
+        <v>20.084468999999999</v>
       </c>
       <c r="K11">
-        <v>-9.0347989999999996</v>
+        <v>-8.1144069999999999</v>
       </c>
       <c r="M11">
-        <v>17.510120000000001</v>
+        <v>17.511465000000001</v>
       </c>
       <c r="N11">
-        <v>-8.924118</v>
+        <v>-7.895543</v>
       </c>
       <c r="P11">
-        <v>15.686230999999999</v>
+        <v>15.785365000000001</v>
       </c>
       <c r="Q11">
-        <v>-8.7600650000000009</v>
+        <v>-7.6774434999999999</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>21.089148000000002</v>
+        <v>21.513978999999999</v>
       </c>
       <c r="B12">
-        <v>-12.013075000000001</v>
+        <v>-10.957814000000001</v>
       </c>
       <c r="D12">
-        <v>22.624227999999999</v>
+        <v>23.048351</v>
       </c>
       <c r="E12">
-        <v>-8.8475280000000005</v>
+        <v>-8.3336240000000004</v>
       </c>
       <c r="G12">
-        <v>22.166256000000001</v>
+        <v>22.265356000000001</v>
       </c>
       <c r="H12">
-        <v>-10.335844</v>
+        <v>-9.2802900000000008</v>
       </c>
       <c r="J12">
-        <v>20.049385000000001</v>
+        <v>20.180986000000001</v>
       </c>
       <c r="K12">
-        <v>-10.036187999999999</v>
+        <v>-9.0347989999999996</v>
       </c>
       <c r="M12">
-        <v>17.541422000000001</v>
+        <v>17.510120000000001</v>
       </c>
       <c r="N12">
-        <v>-9.8985859999999999</v>
+        <v>-8.924118</v>
       </c>
       <c r="P12">
-        <v>15.717530999999999</v>
+        <v>15.686230999999999</v>
       </c>
       <c r="Q12">
-        <v>-9.734534</v>
+        <v>-8.7600650000000009</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
+        <v>21.089148000000002</v>
+      </c>
+      <c r="B13">
+        <v>-12.013075000000001</v>
+      </c>
+      <c r="D13">
+        <v>22.624227999999999</v>
+      </c>
+      <c r="E13">
+        <v>-8.8475280000000005</v>
+      </c>
+      <c r="G13">
+        <v>22.166256000000001</v>
+      </c>
+      <c r="H13">
+        <v>-10.335844</v>
+      </c>
+      <c r="J13">
+        <v>20.049385000000001</v>
+      </c>
+      <c r="K13">
+        <v>-10.036187999999999</v>
+      </c>
+      <c r="M13">
+        <v>17.541422000000001</v>
+      </c>
+      <c r="N13">
+        <v>-9.8985859999999999</v>
+      </c>
+      <c r="P13">
+        <v>15.717530999999999</v>
+      </c>
+      <c r="Q13">
+        <v>-9.734534</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>20.597860000000001</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>-14.069784</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <v>22.590451999999999</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>-9.7678030000000007</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>22.425498999999999</v>
       </c>
-      <c r="H13">
+      <c r="H14">
         <v>-11.364654</v>
       </c>
-      <c r="J13">
+      <c r="J14">
         <v>19.982965</v>
       </c>
-      <c r="K13">
+      <c r="K14">
         <v>-11.010569</v>
       </c>
-      <c r="M13">
+      <c r="M14">
         <v>17.409818999999999</v>
       </c>
-      <c r="N13">
+      <c r="N14">
         <v>-10.899976000000001</v>
       </c>
-      <c r="P13">
+      <c r="P14">
         <v>15.585965</v>
       </c>
-      <c r="Q13">
+      <c r="Q14">
         <v>-10.708856000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="D14">
-        <v>22.458850000000002</v>
-      </c>
-      <c r="E14">
-        <v>-10.769193</v>
-      </c>
-      <c r="J14">
-        <v>20.014265000000002</v>
-      </c>
-      <c r="K14">
-        <v>-11.985037999999999</v>
-      </c>
-      <c r="M14">
-        <v>17.40851</v>
-      </c>
-      <c r="N14">
-        <v>-11.901483000000001</v>
-      </c>
-      <c r="P14">
-        <v>15.649768</v>
-      </c>
-      <c r="Q14">
-        <v>-11.737489999999999</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D15">
-        <v>22.229493999999999</v>
+        <v>22.458850000000002</v>
       </c>
       <c r="E15">
-        <v>-11.797561999999999</v>
+        <v>-10.769193</v>
       </c>
       <c r="J15">
-        <v>20.045458</v>
+        <v>20.014265000000002</v>
       </c>
       <c r="K15">
-        <v>-13.0407095</v>
+        <v>-11.985037999999999</v>
       </c>
       <c r="M15">
-        <v>17.342020000000002</v>
+        <v>17.40851</v>
       </c>
       <c r="N15">
-        <v>-12.929999</v>
+        <v>-11.901483000000001</v>
       </c>
       <c r="P15">
-        <v>15.843899</v>
+        <v>15.649768</v>
       </c>
       <c r="Q15">
-        <v>-12.739172999999999</v>
+        <v>-11.737489999999999</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D16">
-        <v>22.000171999999999</v>
+        <v>22.229493999999999</v>
       </c>
       <c r="E16">
-        <v>-12.798863000000001</v>
+        <v>-11.797561999999999</v>
       </c>
       <c r="J16">
-        <v>20.109933999999999</v>
+        <v>20.045458</v>
       </c>
       <c r="K16">
-        <v>-13.555056</v>
+        <v>-13.0407095</v>
       </c>
       <c r="M16">
-        <v>17.92689</v>
+        <v>17.342020000000002</v>
       </c>
       <c r="N16">
-        <v>-14.040305999999999</v>
+        <v>-12.929999</v>
       </c>
       <c r="P16">
-        <v>15.810052000000001</v>
+        <v>15.843899</v>
       </c>
       <c r="Q16">
-        <v>-13.713583</v>
+        <v>-12.739172999999999</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D17">
+        <v>22.000171999999999</v>
+      </c>
+      <c r="E17">
+        <v>-12.798863000000001</v>
+      </c>
+      <c r="J17">
+        <v>20.109933999999999</v>
+      </c>
+      <c r="K17">
+        <v>-13.555056</v>
+      </c>
+      <c r="M17">
+        <v>17.92689</v>
+      </c>
+      <c r="N17">
+        <v>-14.040305999999999</v>
+      </c>
+      <c r="P17">
+        <v>15.810052000000001</v>
+      </c>
+      <c r="Q17">
+        <v>-13.713583</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D18">
         <v>21.835713999999999</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>-14.016764999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>9</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>10</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>11</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J21" t="s">
         <v>12</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M21" t="s">
         <v>13</v>
       </c>
-      <c r="P20" t="s">
+      <c r="P21" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>13.515459</v>
-      </c>
-      <c r="B21">
-        <v>0.14719583</v>
-      </c>
-      <c r="D21">
-        <v>14.558051000000001</v>
-      </c>
-      <c r="E21">
-        <v>0.33572965999999999</v>
-      </c>
-      <c r="G21">
-        <v>15.861015999999999</v>
-      </c>
-      <c r="H21">
-        <v>0.36162186000000002</v>
-      </c>
-      <c r="M21">
-        <v>19.671945999999998</v>
-      </c>
-      <c r="N21">
-        <v>0.24991223000000001</v>
-      </c>
-      <c r="P21">
-        <v>21.234929999999999</v>
-      </c>
-      <c r="Q21">
-        <v>-0.15751482999999999</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>13.514787</v>
+        <v>13.515459</v>
       </c>
       <c r="B22">
-        <v>-0.36709156999999998</v>
+        <v>0.14719583</v>
       </c>
       <c r="D22">
-        <v>14.557414</v>
+        <v>14.558051000000001</v>
       </c>
       <c r="E22">
-        <v>-0.15148997</v>
+        <v>0.33572965999999999</v>
       </c>
       <c r="G22">
-        <v>15.860309000000001</v>
+        <v>15.861015999999999</v>
       </c>
       <c r="H22">
-        <v>-0.17973330000000001</v>
+        <v>0.36162186000000002</v>
       </c>
       <c r="M22">
-        <v>19.671202000000001</v>
+        <v>19.671945999999998</v>
       </c>
       <c r="N22">
-        <v>-0.31851067999999999</v>
+        <v>0.24991223000000001</v>
       </c>
       <c r="P22">
-        <v>21.23433</v>
+        <v>21.234929999999999</v>
       </c>
       <c r="Q22">
-        <v>-0.61766670000000001</v>
+        <v>-0.15751482999999999</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>13.480869999999999</v>
+        <v>13.514787</v>
       </c>
       <c r="B23">
-        <v>-1.3956369</v>
+        <v>-0.36709156999999998</v>
       </c>
       <c r="D23">
-        <v>14.588642999999999</v>
+        <v>14.557414</v>
       </c>
       <c r="E23">
-        <v>-1.1800941</v>
+        <v>-0.15148997</v>
       </c>
       <c r="G23">
-        <v>15.793854</v>
+        <v>15.860309000000001</v>
       </c>
       <c r="H23">
-        <v>-1.1811815999999999</v>
+        <v>-0.17973330000000001</v>
       </c>
       <c r="M23">
-        <v>19.669964</v>
+        <v>19.671202000000001</v>
       </c>
       <c r="N23">
-        <v>-1.2658821</v>
+        <v>-0.31851067999999999</v>
       </c>
       <c r="P23">
-        <v>21.200447</v>
+        <v>21.23433</v>
       </c>
       <c r="Q23">
-        <v>-1.6191443000000001</v>
+        <v>-0.61766670000000001</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>13.479597</v>
+        <v>13.480869999999999</v>
       </c>
       <c r="B24">
-        <v>-2.3700762000000002</v>
+        <v>-1.3956369</v>
       </c>
       <c r="D24">
-        <v>14.587334999999999</v>
+        <v>14.588642999999999</v>
       </c>
       <c r="E24">
-        <v>-2.1816013000000001</v>
+        <v>-1.1800941</v>
       </c>
       <c r="G24">
-        <v>15.662288</v>
+        <v>15.793854</v>
       </c>
       <c r="H24">
-        <v>-2.1555032999999999</v>
+        <v>-1.1811815999999999</v>
       </c>
       <c r="M24">
-        <v>19.342817</v>
+        <v>19.669964</v>
       </c>
       <c r="N24">
-        <v>-2.3482984999999998</v>
+        <v>-1.2658821</v>
       </c>
       <c r="P24">
-        <v>21.231676</v>
+        <v>21.200447</v>
       </c>
       <c r="Q24">
-        <v>-2.6477485000000001</v>
+        <v>-1.6191443000000001</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>13.380568500000001</v>
+        <v>13.479597</v>
       </c>
       <c r="B25">
-        <v>-3.3714949999999999</v>
+        <v>-2.3700762000000002</v>
       </c>
       <c r="D25">
-        <v>14.423124</v>
+        <v>14.587334999999999</v>
       </c>
       <c r="E25">
-        <v>-3.2100290999999999</v>
+        <v>-2.1816013000000001</v>
       </c>
       <c r="G25">
-        <v>15.335210999999999</v>
+        <v>15.662288</v>
       </c>
       <c r="H25">
-        <v>-3.1837841999999998</v>
+        <v>-2.1555032999999999</v>
       </c>
       <c r="M25">
-        <v>18.885483000000001</v>
+        <v>19.342817</v>
       </c>
       <c r="N25">
-        <v>-3.3493940000000002</v>
+        <v>-2.3482984999999998</v>
       </c>
       <c r="P25">
-        <v>21.165151999999999</v>
+        <v>21.231676</v>
       </c>
       <c r="Q25">
-        <v>-3.7033322000000002</v>
+        <v>-2.6477485000000001</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>13.379225</v>
+        <v>13.380568500000001</v>
       </c>
       <c r="B26">
-        <v>-4.4000697000000004</v>
+        <v>-3.3714949999999999</v>
       </c>
       <c r="D26">
-        <v>14.486998</v>
+        <v>14.423124</v>
       </c>
       <c r="E26">
-        <v>-4.1845270000000001</v>
+        <v>-3.2100290999999999</v>
       </c>
       <c r="G26">
-        <v>15.301365000000001</v>
+        <v>15.335210999999999</v>
       </c>
       <c r="H26">
-        <v>-4.1581939999999999</v>
+        <v>-3.1837841999999998</v>
       </c>
       <c r="M26">
-        <v>18.656126</v>
+        <v>18.885483000000001</v>
       </c>
       <c r="N26">
-        <v>-4.3777632999999998</v>
+        <v>-3.3493940000000002</v>
       </c>
       <c r="P26">
-        <v>21.261526</v>
+        <v>21.165151999999999</v>
       </c>
       <c r="Q26">
-        <v>-4.7319950000000004</v>
+        <v>-3.7033322000000002</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>13.312768999999999</v>
+        <v>13.379225</v>
       </c>
       <c r="B27">
-        <v>-5.4015183000000002</v>
+        <v>-4.4000697000000004</v>
       </c>
       <c r="D27">
-        <v>14.420507000000001</v>
+        <v>14.486998</v>
       </c>
       <c r="E27">
-        <v>-5.2130429999999999</v>
+        <v>-4.1845270000000001</v>
       </c>
       <c r="G27">
-        <v>15.234874</v>
+        <v>15.301365000000001</v>
       </c>
       <c r="H27">
-        <v>-5.1867099999999997</v>
+        <v>-4.1581939999999999</v>
       </c>
       <c r="M27">
-        <v>18.459379999999999</v>
+        <v>18.656126</v>
       </c>
       <c r="N27">
-        <v>-5.3790940000000003</v>
+        <v>-4.3777632999999998</v>
       </c>
       <c r="P27">
-        <v>21.162497999999999</v>
+        <v>21.261526</v>
       </c>
       <c r="Q27">
-        <v>-5.7334139999999998</v>
+        <v>-4.7319950000000004</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>13.311496</v>
+        <v>13.312768999999999</v>
       </c>
       <c r="B28">
-        <v>-6.3759575000000002</v>
+        <v>-5.4015183000000002</v>
       </c>
       <c r="D28">
-        <v>14.484344999999999</v>
+        <v>14.420507000000001</v>
       </c>
       <c r="E28">
-        <v>-6.2146087000000003</v>
+        <v>-5.2130429999999999</v>
       </c>
       <c r="G28">
-        <v>15.233565</v>
+        <v>15.234874</v>
       </c>
       <c r="H28">
-        <v>-6.1882169999999999</v>
+        <v>-5.1867099999999997</v>
       </c>
       <c r="M28">
-        <v>18.230093</v>
+        <v>18.459379999999999</v>
       </c>
       <c r="N28">
-        <v>-6.3533273000000001</v>
+        <v>-5.3790940000000003</v>
       </c>
       <c r="P28">
-        <v>21.128686999999999</v>
+        <v>21.162497999999999</v>
       </c>
       <c r="Q28">
-        <v>-6.6807559999999997</v>
+        <v>-5.7334139999999998</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>13.310152</v>
+        <v>13.311496</v>
       </c>
       <c r="B29">
-        <v>-7.4045319999999997</v>
+        <v>-6.3759575000000002</v>
       </c>
       <c r="D29">
-        <v>14.320206000000001</v>
+        <v>14.484344999999999</v>
       </c>
       <c r="E29">
-        <v>-7.1889013999999998</v>
+        <v>-6.2146087000000003</v>
       </c>
       <c r="G29">
-        <v>15.167075000000001</v>
+        <v>15.233565</v>
       </c>
       <c r="H29">
-        <v>-7.2167329999999996</v>
+        <v>-6.1882169999999999</v>
       </c>
       <c r="M29">
-        <v>18.163637000000001</v>
+        <v>18.230093</v>
       </c>
       <c r="N29">
-        <v>-7.3547760000000002</v>
+        <v>-6.3533273000000001</v>
       </c>
       <c r="P29">
-        <v>21.062266999999999</v>
+        <v>21.128686999999999</v>
       </c>
       <c r="Q29">
-        <v>-7.6551365999999996</v>
+        <v>-6.6807559999999997</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>13.308844000000001</v>
+        <v>13.310152</v>
       </c>
       <c r="B30">
-        <v>-8.4060389999999998</v>
+        <v>-7.4045319999999997</v>
       </c>
       <c r="D30">
-        <v>14.351470000000001</v>
+        <v>14.320206000000001</v>
       </c>
       <c r="E30">
-        <v>-8.1904369999999993</v>
+        <v>-7.1889013999999998</v>
       </c>
       <c r="G30">
-        <v>15.068152</v>
+        <v>15.167075000000001</v>
       </c>
       <c r="H30">
-        <v>-8.1369489999999995</v>
+        <v>-7.2167329999999996</v>
       </c>
       <c r="M30">
-        <v>17.966958999999999</v>
+        <v>18.163637000000001</v>
       </c>
       <c r="N30">
-        <v>-8.3019704999999995</v>
+        <v>-7.3547760000000002</v>
       </c>
       <c r="P30">
-        <v>20.442032000000001</v>
+        <v>21.062266999999999</v>
       </c>
       <c r="Q30">
-        <v>-8.6831530000000008</v>
+        <v>-7.6551365999999996</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>13.274997000000001</v>
+        <v>13.308844000000001</v>
       </c>
       <c r="B31">
-        <v>-9.3804490000000005</v>
+        <v>-8.4060389999999998</v>
       </c>
       <c r="D31">
-        <v>14.3827</v>
+        <v>14.351470000000001</v>
       </c>
       <c r="E31">
-        <v>-9.219042</v>
+        <v>-8.1904369999999993</v>
       </c>
       <c r="G31">
-        <v>15.099347</v>
+        <v>15.068152</v>
       </c>
       <c r="H31">
-        <v>-9.1926199999999998</v>
+        <v>-8.1369489999999995</v>
       </c>
       <c r="M31">
-        <v>17.020885</v>
+        <v>17.966958999999999</v>
       </c>
       <c r="N31">
-        <v>-9.4108959999999993</v>
+        <v>-8.3019704999999995</v>
       </c>
       <c r="P31">
-        <v>19.235513999999998</v>
+        <v>20.442032000000001</v>
       </c>
       <c r="Q31">
-        <v>-9.6835730000000009</v>
+        <v>-8.6831530000000008</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>13.306262</v>
+        <v>13.274997000000001</v>
       </c>
       <c r="B32">
-        <v>-10.381985999999999</v>
+        <v>-9.3804490000000005</v>
       </c>
       <c r="D32">
-        <v>14.381392</v>
+        <v>14.3827</v>
       </c>
       <c r="E32">
-        <v>-10.220549</v>
+        <v>-9.219042</v>
       </c>
       <c r="G32">
-        <v>15.098038000000001</v>
+        <v>15.099347</v>
       </c>
       <c r="H32">
-        <v>-10.194127999999999</v>
+        <v>-9.1926199999999998</v>
       </c>
       <c r="M32">
-        <v>16.563549999999999</v>
+        <v>17.020885</v>
       </c>
       <c r="N32">
-        <v>-10.411992</v>
+        <v>-9.4108959999999993</v>
       </c>
       <c r="P32">
-        <v>18.159251999999999</v>
+        <v>19.235513999999998</v>
       </c>
       <c r="Q32">
-        <v>-10.711178</v>
+        <v>-9.6835730000000009</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>13.53293</v>
+        <v>13.306262</v>
       </c>
       <c r="B33">
-        <v>-11.410766000000001</v>
+        <v>-10.381985999999999</v>
       </c>
       <c r="D33">
-        <v>14.282363</v>
+        <v>14.381392</v>
       </c>
       <c r="E33">
-        <v>-11.221968</v>
+        <v>-10.220549</v>
       </c>
       <c r="G33">
-        <v>15.096729</v>
+        <v>15.098038000000001</v>
       </c>
       <c r="H33">
-        <v>-11.195634999999999</v>
+        <v>-10.194127999999999</v>
       </c>
       <c r="M33">
-        <v>16.171399999999998</v>
+        <v>16.563549999999999</v>
       </c>
       <c r="N33">
-        <v>-11.386079000000001</v>
+        <v>-10.411992</v>
       </c>
       <c r="P33">
-        <v>17.539051000000001</v>
+        <v>18.159251999999999</v>
       </c>
       <c r="Q33">
-        <v>-11.712127000000001</v>
+        <v>-10.711178</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>13.499048</v>
+        <v>13.53293</v>
       </c>
       <c r="B34">
-        <v>-12.412243999999999</v>
+        <v>-11.410766000000001</v>
       </c>
       <c r="D34">
-        <v>14.476459</v>
+        <v>14.282363</v>
       </c>
       <c r="E34">
-        <v>-12.250719</v>
+        <v>-11.221968</v>
       </c>
       <c r="G34">
-        <v>15.030239</v>
+        <v>15.096729</v>
       </c>
       <c r="H34">
-        <v>-12.224151000000001</v>
+        <v>-11.195634999999999</v>
       </c>
       <c r="M34">
-        <v>16.235130000000002</v>
+        <v>16.171399999999998</v>
       </c>
       <c r="N34">
-        <v>-12.468847999999999</v>
+        <v>-11.386079000000001</v>
       </c>
       <c r="P34">
-        <v>17.439986999999999</v>
+        <v>17.539051000000001</v>
       </c>
       <c r="Q34">
-        <v>-12.740613</v>
+        <v>-11.712127000000001</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35">
+        <v>13.499048</v>
+      </c>
+      <c r="B35">
+        <v>-12.412243999999999</v>
+      </c>
+      <c r="D35">
+        <v>14.476459</v>
+      </c>
+      <c r="E35">
+        <v>-12.250719</v>
+      </c>
+      <c r="G35">
+        <v>15.030239</v>
+      </c>
+      <c r="H35">
+        <v>-12.224151000000001</v>
+      </c>
+      <c r="M35">
+        <v>16.235130000000002</v>
+      </c>
+      <c r="N35">
+        <v>-12.468847999999999</v>
+      </c>
+      <c r="P35">
+        <v>17.439986999999999</v>
+      </c>
+      <c r="Q35">
+        <v>-12.740613</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36">
         <v>13.465166999999999</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <v>-13.413721000000001</v>
       </c>
-      <c r="D35">
+      <c r="D36">
         <v>14.279781</v>
       </c>
-      <c r="E35">
+      <c r="E36">
         <v>-13.197914000000001</v>
       </c>
-      <c r="G35">
+      <c r="G36">
         <v>15.094112000000001</v>
       </c>
-      <c r="H35">
+      <c r="H36">
         <v>-13.198648</v>
       </c>
-      <c r="M35">
+      <c r="M36">
         <v>16.234034999999999</v>
       </c>
-      <c r="N35">
+      <c r="N36">
         <v>-13.307948</v>
       </c>
-      <c r="P35">
+      <c r="P36">
         <v>17.309093000000001</v>
       </c>
-      <c r="Q35">
+      <c r="Q36">
         <v>-13.200647</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="D36">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D37">
         <v>14.279322000000001</v>
       </c>
-      <c r="E36">
+      <c r="E37">
         <v>-13.549795</v>
       </c>
-      <c r="G36">
+      <c r="G37">
         <v>15.061114</v>
       </c>
-      <c r="H36">
+      <c r="H37">
         <v>-13.523433000000001</v>
       </c>
-      <c r="M36">
+      <c r="M37">
         <v>16.103317000000001</v>
       </c>
-      <c r="N36">
+      <c r="N37">
         <v>-13.632644000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
         <v>40544</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D39" s="2">
         <v>40575</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G39" s="2">
         <v>40603</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>24.622264999999999</v>
-      </c>
-      <c r="B39">
-        <v>-0.37711339999999999</v>
-      </c>
-      <c r="D39">
-        <v>27.814373</v>
-      </c>
-      <c r="E39">
-        <v>-0.43412909999999999</v>
-      </c>
-      <c r="G39">
-        <v>24.100845</v>
-      </c>
-      <c r="H39">
-        <v>-0.56611747000000001</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>24.588950000000001</v>
+        <v>24.622264999999999</v>
       </c>
       <c r="B40">
-        <v>-0.94550692999999997</v>
+        <v>-0.37711339999999999</v>
       </c>
       <c r="D40">
-        <v>27.748449999999998</v>
+        <v>27.814373</v>
       </c>
       <c r="E40">
-        <v>-1.0295608999999999</v>
+        <v>-0.43412909999999999</v>
       </c>
       <c r="G40">
-        <v>23.937201999999999</v>
+        <v>24.100845</v>
       </c>
       <c r="H40">
-        <v>-1.1614612</v>
+        <v>-0.56611747000000001</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>24.652930000000001</v>
+        <v>24.588950000000001</v>
       </c>
       <c r="B41">
-        <v>-1.8388017000000001</v>
+        <v>-0.94550692999999997</v>
       </c>
       <c r="D41">
-        <v>27.649491999999999</v>
+        <v>27.748449999999998</v>
       </c>
       <c r="E41">
-        <v>-1.9768443</v>
+        <v>-1.0295608999999999</v>
       </c>
       <c r="G41">
-        <v>23.70795</v>
+        <v>23.937201999999999</v>
       </c>
       <c r="H41">
-        <v>-2.1086269999999998</v>
+        <v>-1.1614612</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>24.619012999999999</v>
+        <v>24.652930000000001</v>
       </c>
       <c r="B42">
-        <v>-2.8673470000000001</v>
+        <v>-1.8388017000000001</v>
       </c>
       <c r="D42">
-        <v>27.452707</v>
+        <v>27.649491999999999</v>
       </c>
       <c r="E42">
-        <v>-3.0052428</v>
+        <v>-1.9768443</v>
       </c>
       <c r="G42">
-        <v>23.739286</v>
+        <v>23.70795</v>
       </c>
       <c r="H42">
-        <v>-3.056028</v>
+        <v>-2.1086269999999998</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>24.552593000000002</v>
+        <v>24.619012999999999</v>
       </c>
       <c r="B43">
-        <v>-3.8417275000000002</v>
+        <v>-2.8673470000000001</v>
       </c>
       <c r="D43">
-        <v>26.409126000000001</v>
+        <v>27.452707</v>
       </c>
       <c r="E43">
-        <v>-3.9516737000000002</v>
+        <v>-3.0052428</v>
       </c>
       <c r="G43">
-        <v>23.705334000000001</v>
+        <v>23.739286</v>
       </c>
       <c r="H43">
-        <v>-4.1116409999999997</v>
+        <v>-3.056028</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>23.964859000000001</v>
+        <v>24.552593000000002</v>
       </c>
       <c r="B44">
-        <v>-4.9239087000000001</v>
+        <v>-3.8417275000000002</v>
       </c>
       <c r="D44">
-        <v>25.821498999999999</v>
+        <v>26.409126000000001</v>
       </c>
       <c r="E44">
-        <v>-4.9526519999999996</v>
+        <v>-3.9516737000000002</v>
       </c>
       <c r="G44">
-        <v>23.671488</v>
+        <v>23.705334000000001</v>
       </c>
       <c r="H44">
-        <v>-5.0860510000000003</v>
+        <v>-4.1116409999999997</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>23.898440000000001</v>
+        <v>23.964859000000001</v>
       </c>
       <c r="B45">
-        <v>-5.8982890000000001</v>
+        <v>-4.9239087000000001</v>
       </c>
       <c r="D45">
-        <v>25.429382</v>
+        <v>25.821498999999999</v>
       </c>
       <c r="E45">
-        <v>-5.8996706000000003</v>
+        <v>-4.9526519999999996</v>
       </c>
       <c r="G45">
-        <v>23.279264000000001</v>
+        <v>23.671488</v>
       </c>
       <c r="H45">
-        <v>-6.1142729999999998</v>
+        <v>-5.0860510000000003</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>23.669083000000001</v>
+        <v>23.898440000000001</v>
       </c>
       <c r="B46">
-        <v>-6.9266585999999997</v>
+        <v>-5.8982890000000001</v>
       </c>
       <c r="D46">
-        <v>24.874258000000001</v>
+        <v>25.429382</v>
       </c>
       <c r="E46">
-        <v>-6.9548135000000002</v>
+        <v>-5.8996706000000003</v>
       </c>
       <c r="G46">
-        <v>23.147734</v>
+        <v>23.279264000000001</v>
       </c>
       <c r="H46">
-        <v>-7.0615269999999999</v>
+        <v>-6.1142729999999998</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>23.407222999999998</v>
+        <v>23.669083000000001</v>
       </c>
       <c r="B47">
-        <v>-7.9008627000000002</v>
+        <v>-6.9266585999999997</v>
       </c>
       <c r="D47">
-        <v>24.645005999999999</v>
+        <v>24.874258000000001</v>
       </c>
       <c r="E47">
-        <v>-7.9019794000000001</v>
+        <v>-6.9548135000000002</v>
       </c>
       <c r="G47">
-        <v>23.081244000000002</v>
+        <v>23.147734</v>
       </c>
       <c r="H47">
-        <v>-8.0900429999999997</v>
+        <v>-7.0615269999999999</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>23.015072</v>
+        <v>23.407222999999998</v>
       </c>
       <c r="B48">
-        <v>-8.8749490000000009</v>
+        <v>-7.9008627000000002</v>
       </c>
       <c r="D48">
-        <v>23.796759000000002</v>
+        <v>24.645005999999999</v>
       </c>
       <c r="E48">
-        <v>-8.9297904999999993</v>
+        <v>-7.9019794000000001</v>
       </c>
       <c r="G48">
-        <v>22.98218</v>
+        <v>23.081244000000002</v>
       </c>
       <c r="H48">
-        <v>-9.1185290000000006</v>
+        <v>-8.0900429999999997</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>22.362297000000002</v>
+        <v>23.015072</v>
       </c>
       <c r="B49">
-        <v>-9.8758689999999998</v>
+        <v>-8.8749490000000009</v>
       </c>
       <c r="D49">
-        <v>23.04616</v>
+        <v>23.796759000000002</v>
       </c>
       <c r="E49">
-        <v>-10.011825</v>
+        <v>-8.9297904999999993</v>
       </c>
       <c r="G49">
-        <v>22.883223000000001</v>
+        <v>22.98218</v>
       </c>
       <c r="H49">
-        <v>-10.065813</v>
+        <v>-9.1185290000000006</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>21.709558000000001</v>
+        <v>22.362297000000002</v>
       </c>
       <c r="B50">
-        <v>-10.84972</v>
+        <v>-9.8758689999999998</v>
       </c>
       <c r="D50">
-        <v>21.513836000000001</v>
+        <v>23.04616</v>
       </c>
       <c r="E50">
-        <v>-11.066086</v>
+        <v>-10.011825</v>
       </c>
       <c r="G50">
-        <v>22.849304</v>
+        <v>22.883223000000001</v>
       </c>
       <c r="H50">
-        <v>-11.094358</v>
+        <v>-10.065813</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>20.437859</v>
+        <v>21.709558000000001</v>
       </c>
       <c r="B51">
-        <v>-11.877148999999999</v>
+        <v>-10.84972</v>
       </c>
       <c r="D51">
-        <v>21.545241999999998</v>
+        <v>21.513836000000001</v>
       </c>
       <c r="E51">
-        <v>-11.959351</v>
+        <v>-11.066086</v>
       </c>
       <c r="G51">
-        <v>22.717669000000001</v>
+        <v>22.849304</v>
       </c>
       <c r="H51">
-        <v>-12.122814999999999</v>
+        <v>-11.094358</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>19.459387</v>
+        <v>20.437859</v>
       </c>
       <c r="B52">
-        <v>-12.850706000000001</v>
+        <v>-11.877148999999999</v>
       </c>
       <c r="D52">
-        <v>21.576508</v>
+        <v>21.545241999999998</v>
       </c>
       <c r="E52">
-        <v>-12.960888000000001</v>
+        <v>-11.959351</v>
       </c>
       <c r="G52">
-        <v>22.358090000000001</v>
+        <v>22.717669000000001</v>
       </c>
       <c r="H52">
-        <v>-13.096931</v>
+        <v>-12.122814999999999</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53">
+        <v>19.459387</v>
+      </c>
+      <c r="B53">
+        <v>-12.850706000000001</v>
+      </c>
+      <c r="D53">
+        <v>21.576508</v>
+      </c>
+      <c r="E53">
+        <v>-12.960888000000001</v>
+      </c>
+      <c r="G53">
+        <v>22.358090000000001</v>
+      </c>
+      <c r="H53">
+        <v>-13.096931</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54">
         <v>19.458856999999998</v>
       </c>
-      <c r="B53">
+      <c r="B54">
         <v>-13.256722</v>
       </c>
-      <c r="D53">
+      <c r="D54">
         <v>21.510370000000002</v>
       </c>
-      <c r="E53">
+      <c r="E54">
         <v>-13.718726</v>
       </c>
-      <c r="G53">
+      <c r="G54">
         <v>22.389885</v>
       </c>
-      <c r="H53">
+      <c r="H54">
         <v>-13.692451500000001</v>
       </c>
     </row>

</xml_diff>